<commit_message>
Refined the fitness function so that it was more tunable to historic data
</commit_message>
<xml_diff>
--- a/fitnessfunctions.xlsx
+++ b/fitnessfunctions.xlsx
@@ -335,154 +335,154 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1926131584804382E-2</c:v>
+                  <c:v>6.2778689842436522E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6039236667726508E-2</c:v>
+                  <c:v>0.12530971431552018</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.8585531463824456E-2</c:v>
+                  <c:v>0.18734638510334298</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.10787596006719916</c:v>
+                  <c:v>0.24864396414235745</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1527021054887692</c:v>
+                  <c:v>0.30896062912643957</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.20205370858917118</c:v>
+                  <c:v>0.3680584275091297</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.25501910708825992</c:v>
+                  <c:v>0.42570421523945878</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.31074216576413605</c:v>
+                  <c:v>0.48167057652799755</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.36840224188466358</c:v>
+                  <c:v>0.53573672101459868</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.42720518844848654</c:v>
+                  <c:v>0.58768935479845996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.48638023235202077</c:v>
+                  <c:v>0.63732352189424268</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.54518020297189163</c:v>
+                  <c:v>0.6844434127946577</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.60288374894871999</c:v>
+                  <c:v>0.72886313694969518</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.65879874577006958</c:v>
+                  <c:v>0.77040745611502337</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.71226639326621899</c:v>
+                  <c:v>0.80891247567646041</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.76266566813392245</c:v>
+                  <c:v>0.84422629122320125</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.80941789496488203</c:v>
+                  <c:v>0.87620958781903735</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.85199126073559717</c:v>
+                  <c:v>0.90473618960740965</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.88990513824587913</c:v>
+                  <c:v>0.92969355758207217</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.92273411222949031</c:v>
+                  <c:v>0.95098323355963443</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.95011162269491345</c:v>
+                  <c:v>0.96852122860248668</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.97173315634691548</c:v>
+                  <c:v>0.98223835435975881</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.9873589304086634</c:v>
+                  <c:v>0.99208049601915282</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.99681602486601706</c:v>
+                  <c:v>0.99800882579284111</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.99999992975234597</c:v>
+                  <c:v>0.99999995609521564</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.99687548400690595</c:v>
+                  <c:v>0.99804603180819418</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.98747719195011552</c:v>
+                  <c:v>0.99215476127009083</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.97190891271664603</c:v>
+                  <c:v>0.9823493858657999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.95034292721822344</c:v>
+                  <c:v>0.9686685883382592</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.92301839650434647</c:v>
+                  <c:v>0.9511663401829108</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.89023923489663215</c:v>
+                  <c:v>0.92991168872719632</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.85237143118223824</c:v>
+                  <c:v>0.90498848473506865</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.8098398617404261</c:v>
+                  <c:v>0.87649505161113617</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.76312465116513395</c:v>
+                  <c:v>0.84454379750944719</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.7127571493947058</c:v>
+                  <c:v>0.80926077187716683</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.65931561061923838</c:v>
+                  <c:v>0.77078516818260501</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.60342068001665827</c:v>
+                  <c:v>0.72926877478936092</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.5457308225163181</c:v>
+                  <c:v>0.68487537614291649</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.48693786817096274</c:v>
+                  <c:v>0.63778010663202966</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.42776290994132338</c:v>
+                  <c:v>0.58816875967398119</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.36895288759982481</c:v>
+                  <c:v>0.53623705474936667</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.31127835660138142</c:v>
+                  <c:v>0.48218986527802948</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.25553323558278024</c:v>
+                  <c:v>0.42624041038219801</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.20253788735250727</c:v>
+                  <c:v>0.36860941372537448</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.1531480421608272</c:v>
+                  <c:v>0.30952423274539381</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.10827468864921881</c:v>
+                  <c:v>0.24921796171687957</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>6.8926826092769067E-2</c:v>
+                  <c:v>0.18792851218156797</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3.631017419328024E-2</c:v>
+                  <c:v>0.12589767437424562</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.210641961027195E-2</c:v>
+                  <c:v>6.3370163347032993E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>6.8624853488454106E-6</c:v>
+                  <c:v>5.9265355510034205E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1585,7 +1585,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1603,11 +1603,11 @@
         <v>0</v>
       </c>
       <c r="D1">
-        <f>POWER(SIN(B1),$E$1)</f>
+        <f>POWER(C1,$E$1)</f>
         <v>0</v>
       </c>
       <c r="E1">
-        <v>1.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1624,8 +1624,8 @@
         <v>6.2778689842436522E-2</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D51" si="2">POWER(SIN(B2),$E$1)</f>
-        <v>1.1926131584804382E-2</v>
+        <f t="shared" ref="D2:D51" si="2">POWER(C2,$E$1)</f>
+        <v>6.2778689842436522E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1643,7 +1643,7 @@
       </c>
       <c r="D3">
         <f t="shared" si="2"/>
-        <v>3.6039236667726508E-2</v>
+        <v>0.12530971431552018</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="D4">
         <f t="shared" si="2"/>
-        <v>6.8585531463824456E-2</v>
+        <v>0.18734638510334298</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1679,7 +1679,7 @@
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
-        <v>0.10787596006719916</v>
+        <v>0.24864396414235745</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1697,7 +1697,7 @@
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
-        <v>0.1527021054887692</v>
+        <v>0.30896062912643957</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1715,7 +1715,7 @@
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
-        <v>0.20205370858917118</v>
+        <v>0.3680584275091297</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1733,7 +1733,7 @@
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>0.25501910708825992</v>
+        <v>0.42570421523945878</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1751,7 +1751,7 @@
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>0.31074216576413605</v>
+        <v>0.48167057652799755</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1769,7 +1769,7 @@
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>0.36840224188466358</v>
+        <v>0.53573672101459868</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1787,7 +1787,7 @@
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>0.42720518844848654</v>
+        <v>0.58768935479845996</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1805,7 +1805,7 @@
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>0.48638023235202077</v>
+        <v>0.63732352189424268</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
-        <v>0.54518020297189163</v>
+        <v>0.6844434127946577</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>0.60288374894871999</v>
+        <v>0.72886313694969518</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1859,7 +1859,7 @@
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
-        <v>0.65879874577006958</v>
+        <v>0.77040745611502337</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1877,7 +1877,7 @@
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
-        <v>0.71226639326621899</v>
+        <v>0.80891247567646041</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1895,7 +1895,7 @@
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
-        <v>0.76266566813392245</v>
+        <v>0.84422629122320125</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
-        <v>0.80941789496488203</v>
+        <v>0.87620958781903735</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1931,7 +1931,7 @@
       </c>
       <c r="D19">
         <f t="shared" si="2"/>
-        <v>0.85199126073559717</v>
+        <v>0.90473618960740965</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1949,7 +1949,7 @@
       </c>
       <c r="D20">
         <f t="shared" si="2"/>
-        <v>0.88990513824587913</v>
+        <v>0.92969355758207217</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1967,7 +1967,7 @@
       </c>
       <c r="D21">
         <f t="shared" si="2"/>
-        <v>0.92273411222949031</v>
+        <v>0.95098323355963443</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1985,7 +1985,7 @@
       </c>
       <c r="D22">
         <f t="shared" si="2"/>
-        <v>0.95011162269491345</v>
+        <v>0.96852122860248668</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2003,7 +2003,7 @@
       </c>
       <c r="D23">
         <f t="shared" si="2"/>
-        <v>0.97173315634691548</v>
+        <v>0.98223835435975881</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2021,7 +2021,7 @@
       </c>
       <c r="D24">
         <f t="shared" si="2"/>
-        <v>0.9873589304086634</v>
+        <v>0.99208049601915282</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2039,7 +2039,7 @@
       </c>
       <c r="D25">
         <f t="shared" si="2"/>
-        <v>0.99681602486601706</v>
+        <v>0.99800882579284111</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2057,7 +2057,7 @@
       </c>
       <c r="D26">
         <f t="shared" si="2"/>
-        <v>0.99999992975234597</v>
+        <v>0.99999995609521564</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2075,7 +2075,7 @@
       </c>
       <c r="D27">
         <f t="shared" si="2"/>
-        <v>0.99687548400690595</v>
+        <v>0.99804603180819418</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2093,7 +2093,7 @@
       </c>
       <c r="D28">
         <f t="shared" si="2"/>
-        <v>0.98747719195011552</v>
+        <v>0.99215476127009083</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2111,7 +2111,7 @@
       </c>
       <c r="D29">
         <f t="shared" si="2"/>
-        <v>0.97190891271664603</v>
+        <v>0.9823493858657999</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="D30">
         <f t="shared" si="2"/>
-        <v>0.95034292721822344</v>
+        <v>0.9686685883382592</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="D31">
         <f t="shared" si="2"/>
-        <v>0.92301839650434647</v>
+        <v>0.9511663401829108</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2165,7 +2165,7 @@
       </c>
       <c r="D32">
         <f t="shared" si="2"/>
-        <v>0.89023923489663215</v>
+        <v>0.92991168872719632</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2183,7 +2183,7 @@
       </c>
       <c r="D33">
         <f t="shared" si="2"/>
-        <v>0.85237143118223824</v>
+        <v>0.90498848473506865</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="D34">
         <f t="shared" si="2"/>
-        <v>0.8098398617404261</v>
+        <v>0.87649505161113617</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2219,7 +2219,7 @@
       </c>
       <c r="D35">
         <f t="shared" si="2"/>
-        <v>0.76312465116513395</v>
+        <v>0.84454379750944719</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2237,7 +2237,7 @@
       </c>
       <c r="D36">
         <f t="shared" si="2"/>
-        <v>0.7127571493947058</v>
+        <v>0.80926077187716683</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2255,7 +2255,7 @@
       </c>
       <c r="D37">
         <f t="shared" si="2"/>
-        <v>0.65931561061923838</v>
+        <v>0.77078516818260501</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2273,7 +2273,7 @@
       </c>
       <c r="D38">
         <f t="shared" si="2"/>
-        <v>0.60342068001665827</v>
+        <v>0.72926877478936092</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2291,7 +2291,7 @@
       </c>
       <c r="D39">
         <f t="shared" si="2"/>
-        <v>0.5457308225163181</v>
+        <v>0.68487537614291649</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2309,7 +2309,7 @@
       </c>
       <c r="D40">
         <f t="shared" si="2"/>
-        <v>0.48693786817096274</v>
+        <v>0.63778010663202966</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2327,7 +2327,7 @@
       </c>
       <c r="D41">
         <f t="shared" si="2"/>
-        <v>0.42776290994132338</v>
+        <v>0.58816875967398119</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2345,7 +2345,7 @@
       </c>
       <c r="D42">
         <f t="shared" si="2"/>
-        <v>0.36895288759982481</v>
+        <v>0.53623705474936667</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="D43">
         <f t="shared" si="2"/>
-        <v>0.31127835660138142</v>
+        <v>0.48218986527802948</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2381,7 +2381,7 @@
       </c>
       <c r="D44">
         <f t="shared" si="2"/>
-        <v>0.25553323558278024</v>
+        <v>0.42624041038219801</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2399,7 +2399,7 @@
       </c>
       <c r="D45">
         <f t="shared" si="2"/>
-        <v>0.20253788735250727</v>
+        <v>0.36860941372537448</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2417,7 +2417,7 @@
       </c>
       <c r="D46">
         <f t="shared" si="2"/>
-        <v>0.1531480421608272</v>
+        <v>0.30952423274539381</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2435,7 +2435,7 @@
       </c>
       <c r="D47">
         <f t="shared" si="2"/>
-        <v>0.10827468864921881</v>
+        <v>0.24921796171687957</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="D48">
         <f t="shared" si="2"/>
-        <v>6.8926826092769067E-2</v>
+        <v>0.18792851218156797</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2471,7 +2471,7 @@
       </c>
       <c r="D49">
         <f t="shared" si="2"/>
-        <v>3.631017419328024E-2</v>
+        <v>0.12589767437424562</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2489,7 +2489,7 @@
       </c>
       <c r="D50">
         <f t="shared" si="2"/>
-        <v>1.210641961027195E-2</v>
+        <v>6.3370163347032993E-2</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2507,7 +2507,7 @@
       </c>
       <c r="D51">
         <f t="shared" si="2"/>
-        <v>6.8624853488454106E-6</v>
+        <v>5.9265355510034205E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed fitness functions so they still work over big genes
</commit_message>
<xml_diff>
--- a/fitnessfunctions.xlsx
+++ b/fitnessfunctions.xlsx
@@ -22,6 +22,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+  <si>
+    <t>SinPi</t>
+  </si>
+  <si>
+    <t>SinPiOver2</t>
+  </si>
+  <si>
+    <t>SinPi 100</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -703,36 +717,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -742,6 +726,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SinPi</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -756,309 +751,309 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$A$1:$A$100</c:f>
+              <c:f>Sheet2!$A$2:$A$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>658</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77</c:v>
+                  <c:v>633</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72</c:v>
+                  <c:v>629</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>77</c:v>
+                  <c:v>648</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51</c:v>
+                  <c:v>599</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>68</c:v>
+                  <c:v>657</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72</c:v>
+                  <c:v>637</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64</c:v>
+                  <c:v>617</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>69</c:v>
+                  <c:v>627</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>65</c:v>
+                  <c:v>656</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>74</c:v>
+                  <c:v>631</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>58</c:v>
+                  <c:v>653</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>63</c:v>
+                  <c:v>640</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>53</c:v>
+                  <c:v>676</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>61</c:v>
+                  <c:v>659</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>67</c:v>
+                  <c:v>688</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>75</c:v>
+                  <c:v>625</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>68</c:v>
+                  <c:v>603</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>59</c:v>
+                  <c:v>649</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>74</c:v>
+                  <c:v>668</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>63</c:v>
+                  <c:v>654</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>70</c:v>
+                  <c:v>679</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>61</c:v>
+                  <c:v>638</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>76</c:v>
+                  <c:v>669</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>64</c:v>
+                  <c:v>633</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>63</c:v>
+                  <c:v>652</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>72</c:v>
+                  <c:v>677</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>53</c:v>
+                  <c:v>647</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>61</c:v>
+                  <c:v>633</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>63</c:v>
+                  <c:v>684</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>66</c:v>
+                  <c:v>669</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>71</c:v>
+                  <c:v>684</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>72</c:v>
+                  <c:v>715</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>68</c:v>
+                  <c:v>686</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>78</c:v>
+                  <c:v>709</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>56</c:v>
+                  <c:v>640</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>61</c:v>
+                  <c:v>690</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>76</c:v>
+                  <c:v>699</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>60</c:v>
+                  <c:v>709</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>69</c:v>
+                  <c:v>689</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>63</c:v>
+                  <c:v>694</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>70</c:v>
+                  <c:v>695</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>72</c:v>
+                  <c:v>715</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>74</c:v>
+                  <c:v>742</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>77</c:v>
+                  <c:v>720</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>65</c:v>
+                  <c:v>709</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>71</c:v>
+                  <c:v>760</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>78</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>81</c:v>
+                  <c:v>675</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>73</c:v>
+                  <c:v>761</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>80</c:v>
+                  <c:v>747</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>89</c:v>
+                  <c:v>789</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>75</c:v>
+                  <c:v>762</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>82</c:v>
+                  <c:v>734</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>81</c:v>
+                  <c:v>778</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>89</c:v>
+                  <c:v>760</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>72</c:v>
+                  <c:v>772</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>87</c:v>
+                  <c:v>772</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>74</c:v>
+                  <c:v>754</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>74</c:v>
+                  <c:v>754</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>92</c:v>
+                  <c:v>802</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>73</c:v>
+                  <c:v>771</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>78</c:v>
+                  <c:v>827</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>74</c:v>
+                  <c:v>880</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>76</c:v>
+                  <c:v>786</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>106</c:v>
+                  <c:v>820</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>86</c:v>
+                  <c:v>835</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>84</c:v>
+                  <c:v>870</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>82</c:v>
+                  <c:v>874</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>79</c:v>
+                  <c:v>851</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>112</c:v>
+                  <c:v>863</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>89</c:v>
+                  <c:v>914</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>93</c:v>
+                  <c:v>908</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>85</c:v>
+                  <c:v>930</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>90</c:v>
+                  <c:v>968</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>84</c:v>
+                  <c:v>972</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>83</c:v>
+                  <c:v>990</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>95</c:v>
+                  <c:v>997</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>87</c:v>
+                  <c:v>1013</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>99</c:v>
+                  <c:v>1014</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>85</c:v>
+                  <c:v>1065</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>95</c:v>
+                  <c:v>1053</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>126</c:v>
+                  <c:v>1116</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>125</c:v>
+                  <c:v>1191</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>135</c:v>
+                  <c:v>1201</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>120</c:v>
+                  <c:v>1178</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>102</c:v>
+                  <c:v>1254</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>124</c:v>
+                  <c:v>1274</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>132</c:v>
+                  <c:v>1421</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>133</c:v>
+                  <c:v>1450</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>147</c:v>
+                  <c:v>1541</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>156</c:v>
+                  <c:v>1614</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>162</c:v>
+                  <c:v>1646</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>204</c:v>
+                  <c:v>1830</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>186</c:v>
+                  <c:v>1927</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>205</c:v>
+                  <c:v>2105</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>256</c:v>
+                  <c:v>2438</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>286</c:v>
+                  <c:v>2882</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>386</c:v>
+                  <c:v>3736</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>916</c:v>
+                  <c:v>9091</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1067,6 +1062,1032 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-82CF-44A2-ADBE-4C56B86FAB15}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SinPiOver2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>656</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>609</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>591</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>654</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>624</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>635</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>677</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>589</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>643</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>606</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>684</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>648</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>632</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>664</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>632</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>632</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>643</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>663</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>689</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>646</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>617</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>682</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>638</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>634</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>637</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>697</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>672</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>678</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>673</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>654</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>668</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>678</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>711</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>656</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>673</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>676</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>715</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>711</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>722</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>788</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>679</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>705</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>778</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>745</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>725</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>778</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>774</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>758</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>764</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>733</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>755</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>801</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>772</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>851</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>838</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>878</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>797</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>848</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>887</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>839</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>876</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>893</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>892</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>938</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>941</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>902</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>943</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>933</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>954</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1022</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1005</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1056</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1063</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1129</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1121</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1172</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1132</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1256</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1240</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1323</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1378</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1401</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1497</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1623</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1713</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1699</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2166</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2386</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2863</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3771</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>9101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-461D-4D93-ACCD-FBB96EE5039C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SinPi 100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$2:$C$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>299</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>341</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>435</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>534</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>541</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>646</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>632</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>714</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>674</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>704</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>746</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>758</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>795</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>818</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>866</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>897</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>904</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>918</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>904</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>938</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>965</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>939</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1017</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1011</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1025</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1056</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1064</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1061</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1084</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1021</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1075</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1111</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1135</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1107</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1137</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1117</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1168</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1138</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1131</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1166</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1214</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1181</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1217</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1157</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1187</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1178</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1158</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1206</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1153</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1185</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1173</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1207</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1265</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1253</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1257</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1283</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1243</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1242</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1266</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1235</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1254</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1294</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1213</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1197</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1247</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1328</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1226</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1227</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1243</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1298</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1197</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1239</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1319</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1261</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1205</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1186</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1246</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1282</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1329</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1257</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1223</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1242</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1282</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-461D-4D93-ACCD-FBB96EE5039C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SinPiOver2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>282</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>327</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>374</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>469</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>551</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>566</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>567</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>618</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>665</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>661</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>662</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>742</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>754</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>726</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>824</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>815</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>851</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>874</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>857</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>921</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>841</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>895</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>927</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>963</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1010</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1013</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1021</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1020</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>996</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>979</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1037</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1047</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1055</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1031</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1081</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1118</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1065</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1152</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1066</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1086</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1132</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1143</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1119</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1114</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1152</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1190</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1187</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1144</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1173</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1202</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1149</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1210</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1162</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1194</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1272</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1297</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1217</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1253</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1227</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1186</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1224</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1266</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1225</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1247</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1216</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1187</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1265</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1277</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1265</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1281</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1209</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1230</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1206</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1296</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1338</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1276</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1306</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1279</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1323</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1290</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1294</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1271</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1205</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1291</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1248</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1215</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1236</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-461D-4D93-ACCD-FBB96EE5039C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2391,16 +3412,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3664,512 +4685,1426 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A100"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A100"/>
+      <selection activeCell="D1" sqref="D1:D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>658</v>
+      </c>
+      <c r="B2">
+        <v>656</v>
+      </c>
+      <c r="C2">
+        <v>41</v>
+      </c>
+      <c r="D2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>633</v>
+      </c>
+      <c r="B3">
+        <v>609</v>
+      </c>
+      <c r="C3">
+        <v>140</v>
+      </c>
+      <c r="D3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>629</v>
+      </c>
+      <c r="B4">
+        <v>591</v>
+      </c>
+      <c r="C4">
+        <v>154</v>
+      </c>
+      <c r="D4">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>648</v>
+      </c>
+      <c r="B5">
+        <v>654</v>
+      </c>
+      <c r="C5">
+        <v>243</v>
+      </c>
+      <c r="D5">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>599</v>
+      </c>
+      <c r="B6">
+        <v>624</v>
+      </c>
+      <c r="C6">
+        <v>299</v>
+      </c>
+      <c r="D6">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>657</v>
+      </c>
+      <c r="B7">
+        <v>635</v>
+      </c>
+      <c r="C7">
+        <v>341</v>
+      </c>
+      <c r="D7">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>637</v>
+      </c>
+      <c r="B8">
+        <v>677</v>
+      </c>
+      <c r="C8">
+        <v>338</v>
+      </c>
+      <c r="D8">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+        <v>617</v>
+      </c>
+      <c r="B9">
+        <v>589</v>
+      </c>
+      <c r="C9">
+        <v>410</v>
+      </c>
+      <c r="D9">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+        <v>627</v>
+      </c>
+      <c r="B10">
+        <v>643</v>
+      </c>
+      <c r="C10">
+        <v>435</v>
+      </c>
+      <c r="D10">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+        <v>656</v>
+      </c>
+      <c r="B11">
+        <v>606</v>
+      </c>
+      <c r="C11">
+        <v>440</v>
+      </c>
+      <c r="D11">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+        <v>631</v>
+      </c>
+      <c r="B12">
+        <v>684</v>
+      </c>
+      <c r="C12">
+        <v>534</v>
+      </c>
+      <c r="D12">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+        <v>653</v>
+      </c>
+      <c r="B13">
+        <v>648</v>
+      </c>
+      <c r="C13">
+        <v>541</v>
+      </c>
+      <c r="D13">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+        <v>640</v>
+      </c>
+      <c r="B14">
+        <v>632</v>
+      </c>
+      <c r="C14">
+        <v>580</v>
+      </c>
+      <c r="D14">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+        <v>676</v>
+      </c>
+      <c r="B15">
+        <v>664</v>
+      </c>
+      <c r="C15">
+        <v>646</v>
+      </c>
+      <c r="D15">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>659</v>
+      </c>
+      <c r="B16">
+        <v>615</v>
+      </c>
+      <c r="C16">
+        <v>630</v>
+      </c>
+      <c r="D16">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>688</v>
+      </c>
+      <c r="B17">
+        <v>632</v>
+      </c>
+      <c r="C17">
+        <v>632</v>
+      </c>
+      <c r="D17">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+        <v>625</v>
+      </c>
+      <c r="B18">
+        <v>632</v>
+      </c>
+      <c r="C18">
+        <v>714</v>
+      </c>
+      <c r="D18">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+      <c r="B19">
+        <v>630</v>
+      </c>
+      <c r="C19">
+        <v>674</v>
+      </c>
+      <c r="D19">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+        <v>649</v>
+      </c>
+      <c r="B20">
+        <v>643</v>
+      </c>
+      <c r="C20">
+        <v>704</v>
+      </c>
+      <c r="D20">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+        <v>668</v>
+      </c>
+      <c r="B21">
+        <v>663</v>
+      </c>
+      <c r="C21">
+        <v>746</v>
+      </c>
+      <c r="D21">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+        <v>654</v>
+      </c>
+      <c r="B22">
+        <v>689</v>
+      </c>
+      <c r="C22">
+        <v>758</v>
+      </c>
+      <c r="D22">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+        <v>679</v>
+      </c>
+      <c r="B23">
+        <v>660</v>
+      </c>
+      <c r="C23">
+        <v>768</v>
+      </c>
+      <c r="D23">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+        <v>638</v>
+      </c>
+      <c r="B24">
+        <v>646</v>
+      </c>
+      <c r="C24">
+        <v>795</v>
+      </c>
+      <c r="D24">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+        <v>669</v>
+      </c>
+      <c r="B25">
+        <v>617</v>
+      </c>
+      <c r="C25">
+        <v>818</v>
+      </c>
+      <c r="D25">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+        <v>633</v>
+      </c>
+      <c r="B26">
+        <v>682</v>
+      </c>
+      <c r="C26">
+        <v>830</v>
+      </c>
+      <c r="D26">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+        <v>652</v>
+      </c>
+      <c r="B27">
+        <v>638</v>
+      </c>
+      <c r="C27">
+        <v>866</v>
+      </c>
+      <c r="D27">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+        <v>677</v>
+      </c>
+      <c r="B28">
+        <v>634</v>
+      </c>
+      <c r="C28">
+        <v>897</v>
+      </c>
+      <c r="D28">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+        <v>647</v>
+      </c>
+      <c r="B29">
+        <v>637</v>
+      </c>
+      <c r="C29">
+        <v>904</v>
+      </c>
+      <c r="D29">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+        <v>633</v>
+      </c>
+      <c r="B30">
+        <v>697</v>
+      </c>
+      <c r="C30">
+        <v>918</v>
+      </c>
+      <c r="D30">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+        <v>684</v>
+      </c>
+      <c r="B31">
+        <v>672</v>
+      </c>
+      <c r="C31">
+        <v>904</v>
+      </c>
+      <c r="D31">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+        <v>669</v>
+      </c>
+      <c r="B32">
+        <v>710</v>
+      </c>
+      <c r="C32">
+        <v>938</v>
+      </c>
+      <c r="D32">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+        <v>684</v>
+      </c>
+      <c r="B33">
+        <v>678</v>
+      </c>
+      <c r="C33">
+        <v>965</v>
+      </c>
+      <c r="D33">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+        <v>715</v>
+      </c>
+      <c r="B34">
+        <v>673</v>
+      </c>
+      <c r="C34">
+        <v>939</v>
+      </c>
+      <c r="D34">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+        <v>686</v>
+      </c>
+      <c r="B35">
+        <v>654</v>
+      </c>
+      <c r="C35">
+        <v>999</v>
+      </c>
+      <c r="D35">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+        <v>709</v>
+      </c>
+      <c r="B36">
+        <v>668</v>
+      </c>
+      <c r="C36">
+        <v>1017</v>
+      </c>
+      <c r="D36">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+        <v>640</v>
+      </c>
+      <c r="B37">
+        <v>678</v>
+      </c>
+      <c r="C37">
+        <v>1011</v>
+      </c>
+      <c r="D37">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+        <v>690</v>
+      </c>
+      <c r="B38">
+        <v>711</v>
+      </c>
+      <c r="C38">
+        <v>980</v>
+      </c>
+      <c r="D38">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+        <v>699</v>
+      </c>
+      <c r="B39">
+        <v>656</v>
+      </c>
+      <c r="C39">
+        <v>1025</v>
+      </c>
+      <c r="D39">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+        <v>709</v>
+      </c>
+      <c r="B40">
+        <v>673</v>
+      </c>
+      <c r="C40">
+        <v>1056</v>
+      </c>
+      <c r="D40">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+        <v>689</v>
+      </c>
+      <c r="B41">
+        <v>676</v>
+      </c>
+      <c r="C41">
+        <v>1064</v>
+      </c>
+      <c r="D41">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+        <v>694</v>
+      </c>
+      <c r="B42">
+        <v>715</v>
+      </c>
+      <c r="C42">
+        <v>1061</v>
+      </c>
+      <c r="D42">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+        <v>695</v>
+      </c>
+      <c r="B43">
+        <v>729</v>
+      </c>
+      <c r="C43">
+        <v>1084</v>
+      </c>
+      <c r="D43">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+        <v>715</v>
+      </c>
+      <c r="B44">
+        <v>711</v>
+      </c>
+      <c r="C44">
+        <v>1021</v>
+      </c>
+      <c r="D44">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+        <v>742</v>
+      </c>
+      <c r="B45">
+        <v>722</v>
+      </c>
+      <c r="C45">
+        <v>1075</v>
+      </c>
+      <c r="D45">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+        <v>720</v>
+      </c>
+      <c r="B46">
+        <v>690</v>
+      </c>
+      <c r="C46">
+        <v>1111</v>
+      </c>
+      <c r="D46">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+        <v>709</v>
+      </c>
+      <c r="B47">
+        <v>788</v>
+      </c>
+      <c r="C47">
+        <v>1135</v>
+      </c>
+      <c r="D47">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+        <v>760</v>
+      </c>
+      <c r="B48">
+        <v>679</v>
+      </c>
+      <c r="C48">
+        <v>1107</v>
+      </c>
+      <c r="D48">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+        <v>700</v>
+      </c>
+      <c r="B49">
+        <v>705</v>
+      </c>
+      <c r="C49">
+        <v>1137</v>
+      </c>
+      <c r="D49">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+        <v>675</v>
+      </c>
+      <c r="B50">
+        <v>778</v>
+      </c>
+      <c r="C50">
+        <v>1100</v>
+      </c>
+      <c r="D50">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+        <v>761</v>
+      </c>
+      <c r="B51">
+        <v>745</v>
+      </c>
+      <c r="C51">
+        <v>1117</v>
+      </c>
+      <c r="D51">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+        <v>747</v>
+      </c>
+      <c r="B52">
+        <v>730</v>
+      </c>
+      <c r="C52">
+        <v>1168</v>
+      </c>
+      <c r="D52">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+        <v>789</v>
+      </c>
+      <c r="B53">
+        <v>725</v>
+      </c>
+      <c r="C53">
+        <v>1138</v>
+      </c>
+      <c r="D53">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+        <v>762</v>
+      </c>
+      <c r="B54">
+        <v>768</v>
+      </c>
+      <c r="C54">
+        <v>1200</v>
+      </c>
+      <c r="D54">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+        <v>734</v>
+      </c>
+      <c r="B55">
+        <v>778</v>
+      </c>
+      <c r="C55">
+        <v>1131</v>
+      </c>
+      <c r="D55">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+        <v>778</v>
+      </c>
+      <c r="B56">
+        <v>774</v>
+      </c>
+      <c r="C56">
+        <v>1166</v>
+      </c>
+      <c r="D56">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+        <v>760</v>
+      </c>
+      <c r="B57">
+        <v>758</v>
+      </c>
+      <c r="C57">
+        <v>1214</v>
+      </c>
+      <c r="D57">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+        <v>772</v>
+      </c>
+      <c r="B58">
+        <v>764</v>
+      </c>
+      <c r="C58">
+        <v>1181</v>
+      </c>
+      <c r="D58">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+        <v>772</v>
+      </c>
+      <c r="B59">
+        <v>733</v>
+      </c>
+      <c r="C59">
+        <v>1217</v>
+      </c>
+      <c r="D59">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+        <v>754</v>
+      </c>
+      <c r="B60">
+        <v>755</v>
+      </c>
+      <c r="C60">
+        <v>1157</v>
+      </c>
+      <c r="D60">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+        <v>754</v>
+      </c>
+      <c r="B61">
+        <v>801</v>
+      </c>
+      <c r="C61">
+        <v>1187</v>
+      </c>
+      <c r="D61">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+        <v>802</v>
+      </c>
+      <c r="B62">
+        <v>772</v>
+      </c>
+      <c r="C62">
+        <v>1178</v>
+      </c>
+      <c r="D62">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+        <v>771</v>
+      </c>
+      <c r="B63">
+        <v>851</v>
+      </c>
+      <c r="C63">
+        <v>1158</v>
+      </c>
+      <c r="D63">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+        <v>827</v>
+      </c>
+      <c r="B64">
+        <v>838</v>
+      </c>
+      <c r="C64">
+        <v>1206</v>
+      </c>
+      <c r="D64">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+        <v>880</v>
+      </c>
+      <c r="B65">
+        <v>878</v>
+      </c>
+      <c r="C65">
+        <v>1153</v>
+      </c>
+      <c r="D65">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="B66">
+        <v>797</v>
+      </c>
+      <c r="C66">
+        <v>1200</v>
+      </c>
+      <c r="D66">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+        <v>820</v>
+      </c>
+      <c r="B67">
+        <v>848</v>
+      </c>
+      <c r="C67">
+        <v>1185</v>
+      </c>
+      <c r="D67">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+        <v>835</v>
+      </c>
+      <c r="B68">
+        <v>887</v>
+      </c>
+      <c r="C68">
+        <v>1173</v>
+      </c>
+      <c r="D68">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+        <v>870</v>
+      </c>
+      <c r="B69">
+        <v>839</v>
+      </c>
+      <c r="C69">
+        <v>1207</v>
+      </c>
+      <c r="D69">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+        <v>874</v>
+      </c>
+      <c r="B70">
+        <v>876</v>
+      </c>
+      <c r="C70">
+        <v>1265</v>
+      </c>
+      <c r="D70">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+        <v>851</v>
+      </c>
+      <c r="B71">
+        <v>893</v>
+      </c>
+      <c r="C71">
+        <v>1253</v>
+      </c>
+      <c r="D71">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+        <v>863</v>
+      </c>
+      <c r="B72">
+        <v>892</v>
+      </c>
+      <c r="C72">
+        <v>1257</v>
+      </c>
+      <c r="D72">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+        <v>914</v>
+      </c>
+      <c r="B73">
+        <v>938</v>
+      </c>
+      <c r="C73">
+        <v>1283</v>
+      </c>
+      <c r="D73">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+        <v>908</v>
+      </c>
+      <c r="B74">
+        <v>941</v>
+      </c>
+      <c r="C74">
+        <v>1300</v>
+      </c>
+      <c r="D74">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+        <v>930</v>
+      </c>
+      <c r="B75">
+        <v>902</v>
+      </c>
+      <c r="C75">
+        <v>1243</v>
+      </c>
+      <c r="D75">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="B76">
+        <v>943</v>
+      </c>
+      <c r="C76">
+        <v>1242</v>
+      </c>
+      <c r="D76">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+        <v>972</v>
+      </c>
+      <c r="B77">
+        <v>933</v>
+      </c>
+      <c r="C77">
+        <v>1266</v>
+      </c>
+      <c r="D77">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+        <v>990</v>
+      </c>
+      <c r="B78">
+        <v>954</v>
+      </c>
+      <c r="C78">
+        <v>1235</v>
+      </c>
+      <c r="D78">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+        <v>997</v>
+      </c>
+      <c r="B79">
+        <v>1022</v>
+      </c>
+      <c r="C79">
+        <v>1254</v>
+      </c>
+      <c r="D79">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1013</v>
+      </c>
+      <c r="B80">
+        <v>1005</v>
+      </c>
+      <c r="C80">
+        <v>1294</v>
+      </c>
+      <c r="D80">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1014</v>
+      </c>
+      <c r="B81">
+        <v>1056</v>
+      </c>
+      <c r="C81">
+        <v>1213</v>
+      </c>
+      <c r="D81">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1065</v>
+      </c>
+      <c r="B82">
+        <v>1063</v>
+      </c>
+      <c r="C82">
+        <v>1197</v>
+      </c>
+      <c r="D82">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1053</v>
+      </c>
+      <c r="B83">
+        <v>1129</v>
+      </c>
+      <c r="C83">
+        <v>1247</v>
+      </c>
+      <c r="D83">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1116</v>
+      </c>
+      <c r="B84">
+        <v>1121</v>
+      </c>
+      <c r="C84">
+        <v>1328</v>
+      </c>
+      <c r="D84">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1191</v>
+      </c>
+      <c r="B85">
+        <v>1172</v>
+      </c>
+      <c r="C85">
+        <v>1226</v>
+      </c>
+      <c r="D85">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1201</v>
+      </c>
+      <c r="B86">
+        <v>1132</v>
+      </c>
+      <c r="C86">
+        <v>1227</v>
+      </c>
+      <c r="D86">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1178</v>
+      </c>
+      <c r="B87">
+        <v>1256</v>
+      </c>
+      <c r="C87">
+        <v>1243</v>
+      </c>
+      <c r="D87">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1254</v>
+      </c>
+      <c r="B88">
+        <v>1240</v>
+      </c>
+      <c r="C88">
+        <v>1298</v>
+      </c>
+      <c r="D88">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1274</v>
+      </c>
+      <c r="B89">
+        <v>1323</v>
+      </c>
+      <c r="C89">
+        <v>1197</v>
+      </c>
+      <c r="D89">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1421</v>
+      </c>
+      <c r="B90">
+        <v>1378</v>
+      </c>
+      <c r="C90">
+        <v>1239</v>
+      </c>
+      <c r="D90">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1450</v>
+      </c>
+      <c r="B91">
+        <v>1401</v>
+      </c>
+      <c r="C91">
+        <v>1319</v>
+      </c>
+      <c r="D91">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1541</v>
+      </c>
+      <c r="B92">
+        <v>1497</v>
+      </c>
+      <c r="C92">
+        <v>1261</v>
+      </c>
+      <c r="D92">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1614</v>
+      </c>
+      <c r="B93">
+        <v>1623</v>
+      </c>
+      <c r="C93">
+        <v>1205</v>
+      </c>
+      <c r="D93">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1646</v>
+      </c>
+      <c r="B94">
+        <v>1713</v>
+      </c>
+      <c r="C94">
+        <v>1186</v>
+      </c>
+      <c r="D94">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1830</v>
+      </c>
+      <c r="B95">
+        <v>1699</v>
+      </c>
+      <c r="C95">
+        <v>1246</v>
+      </c>
+      <c r="D95">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1927</v>
+      </c>
+      <c r="B96">
+        <v>1977</v>
+      </c>
+      <c r="C96">
+        <v>1282</v>
+      </c>
+      <c r="D96">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+        <v>2105</v>
+      </c>
+      <c r="B97">
+        <v>2166</v>
+      </c>
+      <c r="C97">
+        <v>1329</v>
+      </c>
+      <c r="D97">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+        <v>2438</v>
+      </c>
+      <c r="B98">
+        <v>2386</v>
+      </c>
+      <c r="C98">
+        <v>1257</v>
+      </c>
+      <c r="D98">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+        <v>2882</v>
+      </c>
+      <c r="B99">
+        <v>2863</v>
+      </c>
+      <c r="C99">
+        <v>1223</v>
+      </c>
+      <c r="D99">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>916</v>
+        <v>3736</v>
+      </c>
+      <c r="B100">
+        <v>3771</v>
+      </c>
+      <c r="C100">
+        <v>1242</v>
+      </c>
+      <c r="D100">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>9091</v>
+      </c>
+      <c r="B101">
+        <v>9101</v>
+      </c>
+      <c r="C101">
+        <v>1282</v>
+      </c>
+      <c r="D101">
+        <v>1236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>